<commit_message>
Add implementation progress + annual target
</commit_message>
<xml_diff>
--- a/Implementation doc/Mikes_stories.xlsx
+++ b/Implementation doc/Mikes_stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackl\Desktop\Stories for IMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a43712/Desktop/MA.NorwegianBasin/Implementation doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD27C5D-FE41-44EA-9EE6-13E723064563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA031C93-BCAC-074F-B54C-7C9D439ACCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{42E5A92F-267B-4B69-9450-AB0ABF14FAF6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{42E5A92F-267B-4B69-9450-AB0ABF14FAF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tourist1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="118">
   <si>
     <t>Year</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Total annual activity</t>
+  </si>
+  <si>
+    <t>Other regions (78.43% of “North of 62N”)</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -667,6 +670,10 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,9 +692,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -725,7 +732,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -831,7 +838,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -973,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,15 +994,15 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1984</v>
       </c>
@@ -1023,7 +1030,7 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1985</v>
       </c>
@@ -1037,7 +1044,7 @@
         <v>13400</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1986</v>
       </c>
@@ -1051,7 +1058,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1987</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1988</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1989</v>
       </c>
@@ -1093,7 +1100,7 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1990</v>
       </c>
@@ -1107,7 +1114,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1991</v>
       </c>
@@ -1121,7 +1128,7 @@
         <v>15200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1992</v>
       </c>
@@ -1135,7 +1142,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1993</v>
       </c>
@@ -1149,7 +1156,7 @@
         <v>14700</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1994</v>
       </c>
@@ -1163,7 +1170,7 @@
         <v>14600</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1995</v>
       </c>
@@ -1177,7 +1184,7 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1996</v>
       </c>
@@ -1191,7 +1198,7 @@
         <v>14300</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1997</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>14200</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1998</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>14300</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1999</v>
       </c>
@@ -1233,7 +1240,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
@@ -1247,7 +1254,7 @@
         <v>13100</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2001</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>12700</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2002</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>12800</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2003</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2004</v>
       </c>
@@ -1303,7 +1310,7 @@
         <v>12300</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2005</v>
       </c>
@@ -1317,7 +1324,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2006</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>11700</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2007</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>11500</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2008</v>
       </c>
@@ -1359,7 +1366,7 @@
         <v>11200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2009</v>
       </c>
@@ -1373,7 +1380,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2010</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>10810</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2011</v>
       </c>
@@ -1401,7 +1408,7 @@
         <v>10716</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2012</v>
       </c>
@@ -1415,7 +1422,7 @@
         <v>10616</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2013</v>
       </c>
@@ -1429,7 +1436,7 @@
         <v>10512</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2014</v>
       </c>
@@ -1443,7 +1450,7 @@
         <v>10403</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2015</v>
       </c>
@@ -1457,7 +1464,7 @@
         <v>10288</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2016</v>
       </c>
@@ -1471,7 +1478,7 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2017</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>10041</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2018</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>9908</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2019</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>9768</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>2</v>
       </c>
@@ -1541,13 +1548,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.86328125" customWidth="1"/>
-    <col min="2" max="2" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1563,7 +1570,7 @@
         <v>94641</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="46.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>33489</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1587,7 +1594,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>105</v>
       </c>
@@ -1609,9 +1616,9 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>33</v>
       </c>
@@ -1622,7 +1629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>3</v>
       </c>
@@ -1633,7 +1640,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
         <v>4</v>
       </c>
@@ -1644,7 +1651,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>5</v>
       </c>
@@ -1655,7 +1662,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>0</v>
       </c>
@@ -1666,7 +1673,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>6</v>
       </c>
@@ -1677,7 +1684,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
         <v>7</v>
       </c>
@@ -1688,7 +1695,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>28</v>
       </c>
@@ -1699,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
         <v>8</v>
       </c>
@@ -1710,7 +1717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1721,7 +1728,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="38.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>36</v>
       </c>
@@ -1732,7 +1739,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="38.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>37</v>
       </c>
@@ -1743,7 +1750,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" ht="71" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>38</v>
       </c>
@@ -1765,13 +1772,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.796875" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>77</v>
       </c>
@@ -1782,7 +1789,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>41</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>42</v>
       </c>
@@ -1804,7 +1811,7 @@
         <v>0.3372</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>43</v>
       </c>
@@ -1815,7 +1822,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>44</v>
       </c>
@@ -1826,7 +1833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>45</v>
       </c>
@@ -1850,12 +1857,12 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -1863,7 +1870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -1871,7 +1878,7 @@
         <v>94641</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1879,7 +1886,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1887,7 +1894,7 @@
         <v>33489</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>105</v>
       </c>
@@ -1908,13 +1915,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>48</v>
       </c>
@@ -1946,7 +1953,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="20.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -1978,7 +1985,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="20.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>2</v>
       </c>
@@ -2010,7 +2017,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="20.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
         <v>3</v>
       </c>
@@ -2042,7 +2049,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="71.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" ht="85" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -2074,7 +2081,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>5</v>
       </c>
@@ -2106,7 +2113,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30">
         <v>6</v>
       </c>
@@ -2138,7 +2145,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>8</v>
       </c>
@@ -2202,7 +2209,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>9</v>
       </c>
@@ -2247,12 +2254,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>68</v>
       </c>
@@ -2260,7 +2267,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>70</v>
       </c>
@@ -2268,7 +2275,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>71</v>
       </c>
@@ -2276,7 +2283,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>72</v>
       </c>
@@ -2284,7 +2291,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>73</v>
       </c>
@@ -2292,7 +2299,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>107</v>
       </c>
@@ -2300,7 +2307,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>106</v>
       </c>
@@ -2321,12 +2328,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.06640625" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -2337,7 +2344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -2348,7 +2355,7 @@
         <v>169675</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
@@ -2359,7 +2366,7 @@
         <v>3453</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>382537</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>7784</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>105</v>
       </c>
@@ -2399,15 +2406,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4579D33F-77C7-4CB2-BF6A-4CC354C354D6}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="81.75" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="92" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>77</v>
       </c>
@@ -2420,8 +2430,15 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="40">
+        <f>34/52</f>
+        <v>0.65384615384615385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -2434,8 +2451,13 @@
       <c r="D2" s="4">
         <v>335.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E2">
+        <f>0.7843*B2</f>
+        <v>1243.8997999999999</v>
+      </c>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -2448,8 +2470,12 @@
       <c r="D3" s="4">
         <v>24.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="0">0.7843*B3</f>
+        <v>90.272929999999988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -2462,8 +2488,12 @@
       <c r="D4" s="4">
         <v>174.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>647.20436000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -2476,8 +2506,12 @@
       <c r="D5" s="4">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>63.606729999999992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2490,8 +2524,12 @@
       <c r="D6" s="4">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>62.508710000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2504,8 +2542,12 @@
       <c r="D7" s="4">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10.66648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2518,8 +2560,12 @@
       <c r="D8" s="4">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>53.724550000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2532,8 +2578,12 @@
       <c r="D9" s="4">
         <v>36.700000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>136.23291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
@@ -2546,8 +2596,12 @@
       <c r="D10" s="4">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>11.999790000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2560,8 +2614,12 @@
       <c r="D11" s="4">
         <v>625.79999999999995</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="46.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E11">
+        <f>SUM(E2:E10)</f>
+        <v>2320.1162599999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -2574,8 +2632,12 @@
       <c r="D12" s="4">
         <v>622.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="46.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E12">
+        <f>E11-E7</f>
+        <v>2309.4497799999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -2588,8 +2650,12 @@
       <c r="D13" s="4">
         <v>1.857</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="E13">
+        <f>SUM(E2:E6,E8:E10)/E2</f>
+        <v>1.8566204287515764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -2601,6 +2667,10 @@
       </c>
       <c r="D14" s="4">
         <v>8.5800000000000008E-3</v>
+      </c>
+      <c r="E14">
+        <f>E7/E2</f>
+        <v>8.575031525851198E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2612,13 +2682,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72D6535-9D03-4F63-8CAD-8654C9A9FD35}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2647,7 +2717,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1984</v>
       </c>
@@ -2676,7 +2746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1985</v>
       </c>
@@ -2705,7 +2775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1986</v>
       </c>
@@ -2734,7 +2804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1987</v>
       </c>
@@ -2763,7 +2833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1988</v>
       </c>
@@ -2792,7 +2862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1989</v>
       </c>
@@ -2821,7 +2891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1990</v>
       </c>
@@ -2850,7 +2920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1991</v>
       </c>
@@ -2879,7 +2949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1992</v>
       </c>
@@ -2908,7 +2978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1993</v>
       </c>
@@ -2937,7 +3007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1994</v>
       </c>
@@ -2966,7 +3036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1995</v>
       </c>
@@ -2995,7 +3065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1996</v>
       </c>
@@ -3024,7 +3094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1997</v>
       </c>
@@ -3053,7 +3123,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1998</v>
       </c>
@@ -3082,7 +3152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1999</v>
       </c>
@@ -3111,7 +3181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
@@ -3140,7 +3210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2001</v>
       </c>
@@ -3169,7 +3239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2002</v>
       </c>
@@ -3198,7 +3268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2003</v>
       </c>
@@ -3227,7 +3297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2004</v>
       </c>
@@ -3256,7 +3326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2005</v>
       </c>
@@ -3285,7 +3355,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2006</v>
       </c>
@@ -3314,7 +3384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2007</v>
       </c>
@@ -3343,7 +3413,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2008</v>
       </c>
@@ -3372,7 +3442,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:9" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2009</v>
       </c>
@@ -3401,7 +3471,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2010</v>
       </c>
@@ -3430,7 +3500,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2011</v>
       </c>
@@ -3459,7 +3529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2012</v>
       </c>
@@ -3488,7 +3558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2013</v>
       </c>
@@ -3517,7 +3587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2014</v>
       </c>
@@ -3546,7 +3616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2015</v>
       </c>
@@ -3575,7 +3645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2016</v>
       </c>
@@ -3604,7 +3674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2017</v>
       </c>
@@ -3633,7 +3703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2018</v>
       </c>
@@ -3662,7 +3732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2019</v>
       </c>
@@ -3691,7 +3761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>2</v>
       </c>
@@ -3733,12 +3803,12 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="32.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3752,7 +3822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1984</v>
       </c>
@@ -3766,7 +3836,7 @@
         <v>588492</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1985</v>
       </c>
@@ -3780,7 +3850,7 @@
         <v>592917</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>1986</v>
       </c>
@@ -3794,7 +3864,7 @@
         <v>597342</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>1987</v>
       </c>
@@ -3808,7 +3878,7 @@
         <v>597342</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>1988</v>
       </c>
@@ -3822,7 +3892,7 @@
         <v>601767</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>1989</v>
       </c>
@@ -3836,7 +3906,7 @@
         <v>606191</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>1990</v>
       </c>
@@ -3850,7 +3920,7 @@
         <v>641589</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>1991</v>
       </c>
@@ -3864,7 +3934,7 @@
         <v>676987</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>1992</v>
       </c>
@@ -3878,7 +3948,7 @@
         <v>712385</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>1993</v>
       </c>
@@ -3892,7 +3962,7 @@
         <v>654864</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>1994</v>
       </c>
@@ -3906,7 +3976,7 @@
         <v>650439</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>1995</v>
       </c>
@@ -3920,7 +3990,7 @@
         <v>650439</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>1996</v>
       </c>
@@ -3934,7 +4004,7 @@
         <v>641589</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>1997</v>
       </c>
@@ -3948,7 +4018,7 @@
         <v>641589</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>1998</v>
       </c>
@@ -3962,7 +4032,7 @@
         <v>646014</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>1999</v>
       </c>
@@ -3976,7 +4046,7 @@
         <v>615041</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>2000</v>
       </c>
@@ -3990,7 +4060,7 @@
         <v>601767</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>2001</v>
       </c>
@@ -4004,7 +4074,7 @@
         <v>592917</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>2002</v>
       </c>
@@ -4018,7 +4088,7 @@
         <v>601767</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>2003</v>
       </c>
@@ -4032,7 +4102,7 @@
         <v>615041</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>2004</v>
       </c>
@@ -4046,7 +4116,7 @@
         <v>592917</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>2005</v>
       </c>
@@ -4060,7 +4130,7 @@
         <v>584068</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>2006</v>
       </c>
@@ -4074,7 +4144,7 @@
         <v>575218</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>2007</v>
       </c>
@@ -4088,7 +4158,7 @@
         <v>575218</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>2008</v>
       </c>
@@ -4102,7 +4172,7 @@
         <v>566368</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>2009</v>
       </c>
@@ -4116,7 +4186,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>2010</v>
       </c>
@@ -4130,7 +4200,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>2011</v>
       </c>
@@ -4144,7 +4214,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>2012</v>
       </c>
@@ -4158,7 +4228,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>2013</v>
       </c>
@@ -4172,7 +4242,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>2014</v>
       </c>
@@ -4186,7 +4256,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>2015</v>
       </c>
@@ -4200,7 +4270,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>2016</v>
       </c>
@@ -4214,7 +4284,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>2017</v>
       </c>
@@ -4228,7 +4298,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>2018</v>
       </c>
@@ -4242,7 +4312,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>2019</v>
       </c>
@@ -4256,7 +4326,7 @@
         <v>561944</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>2</v>
       </c>
@@ -4279,16 +4349,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8184A196-3B4F-4787-8F9F-796845CDFCE1}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4314,7 +4384,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1984</v>
       </c>
@@ -4340,7 +4410,7 @@
         <v>179522</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1985</v>
       </c>
@@ -4366,7 +4436,7 @@
         <v>210743</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1986</v>
       </c>
@@ -4392,7 +4462,7 @@
         <v>144398</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1987</v>
       </c>
@@ -4418,7 +4488,7 @@
         <v>136593</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1988</v>
       </c>
@@ -4444,7 +4514,7 @@
         <v>113177</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1989</v>
       </c>
@@ -4470,7 +4540,7 @@
         <v>156106</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1990</v>
       </c>
@@ -4496,7 +4566,7 @@
         <v>132690</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1991</v>
       </c>
@@ -4522,7 +4592,7 @@
         <v>370752</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1992</v>
       </c>
@@ -4548,7 +4618,7 @@
         <v>897610</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1993</v>
       </c>
@@ -4574,7 +4644,7 @@
         <v>718088</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1994</v>
       </c>
@@ -4600,7 +4670,7 @@
         <v>616619</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1995</v>
       </c>
@@ -4626,7 +4696,7 @@
         <v>538566</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1996</v>
       </c>
@@ -4652,7 +4722,7 @@
         <v>577593</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1997</v>
       </c>
@@ -4678,7 +4748,7 @@
         <v>530761</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1998</v>
       </c>
@@ -4704,7 +4774,7 @@
         <v>507345</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1999</v>
       </c>
@@ -4730,7 +4800,7 @@
         <v>480026</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
@@ -4756,7 +4826,7 @@
         <v>522955</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2001</v>
       </c>
@@ -4782,7 +4852,7 @@
         <v>624424</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2002</v>
       </c>
@@ -4808,7 +4878,7 @@
         <v>850778</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2003</v>
       </c>
@@ -4834,7 +4904,7 @@
         <v>601008</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2004</v>
       </c>
@@ -4860,7 +4930,7 @@
         <v>401973</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2005</v>
       </c>
@@ -4886,7 +4956,7 @@
         <v>404315</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2006</v>
       </c>
@@ -4912,7 +4982,7 @@
         <v>421486</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2007</v>
       </c>
@@ -4938,7 +5008,7 @@
         <v>460513</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2008</v>
       </c>
@@ -4964,7 +5034,7 @@
         <v>460513</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2009</v>
       </c>
@@ -4990,7 +5060,7 @@
         <v>569787</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2010</v>
       </c>
@@ -5016,7 +5086,7 @@
         <v>690769</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2011</v>
       </c>
@@ -5042,7 +5112,7 @@
         <v>686867</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2012</v>
       </c>
@@ -5068,7 +5138,7 @@
         <v>671256</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2013</v>
       </c>
@@ -5094,7 +5164,7 @@
         <v>757115</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2014</v>
       </c>
@@ -5120,7 +5190,7 @@
         <v>663451</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>21</v>
       </c>
@@ -5159,9 +5229,9 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="66" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5178,7 +5248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1984</v>
       </c>
@@ -5195,7 +5265,7 @@
         <v>768014</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1985</v>
       </c>
@@ -5212,7 +5282,7 @@
         <v>803660</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1986</v>
       </c>
@@ -5229,7 +5299,7 @@
         <v>741740</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1987</v>
       </c>
@@ -5246,7 +5316,7 @@
         <v>733935</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1988</v>
       </c>
@@ -5263,7 +5333,7 @@
         <v>714943</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1989</v>
       </c>
@@ -5280,7 +5350,7 @@
         <v>762297</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1990</v>
       </c>
@@ -5297,7 +5367,7 @@
         <v>774279</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1991</v>
       </c>
@@ -5314,7 +5384,7 @@
         <v>1047739</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1992</v>
       </c>
@@ -5331,7 +5401,7 @@
         <v>1609995</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1993</v>
       </c>
@@ -5348,7 +5418,7 @@
         <v>1372952</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1994</v>
       </c>
@@ -5365,7 +5435,7 @@
         <v>1267058</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1995</v>
       </c>
@@ -5382,7 +5452,7 @@
         <v>1189005</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1996</v>
       </c>
@@ -5399,7 +5469,7 @@
         <v>1219182</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1997</v>
       </c>
@@ -5416,7 +5486,7 @@
         <v>1172350</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1998</v>
       </c>
@@ -5433,7 +5503,7 @@
         <v>1153359</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1999</v>
       </c>
@@ -5450,7 +5520,7 @@
         <v>1095067</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
@@ -5467,7 +5537,7 @@
         <v>1124722</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2001</v>
       </c>
@@ -5484,7 +5554,7 @@
         <v>1217341</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2002</v>
       </c>
@@ -5501,7 +5571,7 @@
         <v>1452545</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2003</v>
       </c>
@@ -5518,7 +5588,7 @@
         <v>1216049</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2004</v>
       </c>
@@ -5535,7 +5605,7 @@
         <v>994890</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2005</v>
       </c>
@@ -5552,7 +5622,7 @@
         <v>988382</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2006</v>
       </c>
@@ -5569,7 +5639,7 @@
         <v>996704</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2007</v>
       </c>
@@ -5586,7 +5656,7 @@
         <v>1035731</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2008</v>
       </c>
@@ -5603,7 +5673,7 @@
         <v>1026881</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2009</v>
       </c>
@@ -5620,7 +5690,7 @@
         <v>1131731</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2010</v>
       </c>
@@ -5637,7 +5707,7 @@
         <v>1252713</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2011</v>
       </c>
@@ -5654,7 +5724,7 @@
         <v>1248811</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2012</v>
       </c>
@@ -5671,7 +5741,7 @@
         <v>1233200</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2013</v>
       </c>
@@ -5688,7 +5758,7 @@
         <v>1319058</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2014</v>
       </c>
@@ -5705,7 +5775,7 @@
         <v>1225395</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2015</v>
       </c>
@@ -5722,7 +5792,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2016</v>
       </c>
@@ -5739,7 +5809,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2017</v>
       </c>
@@ -5756,7 +5826,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2018</v>
       </c>
@@ -5773,7 +5843,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2019</v>
       </c>
@@ -5790,7 +5860,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>21</v>
       </c>
@@ -5820,9 +5890,9 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5839,7 +5909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1994</v>
       </c>
@@ -5856,7 +5926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1995</v>
       </c>
@@ -5873,7 +5943,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1996</v>
       </c>
@@ -5890,7 +5960,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1997</v>
       </c>
@@ -5907,7 +5977,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1998</v>
       </c>
@@ -5924,7 +5994,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1999</v>
       </c>
@@ -5941,7 +6011,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2000</v>
       </c>
@@ -5958,7 +6028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -5975,7 +6045,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2002</v>
       </c>
@@ -5992,7 +6062,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2003</v>
       </c>
@@ -6009,7 +6079,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2004</v>
       </c>
@@ -6026,7 +6096,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2005</v>
       </c>
@@ -6043,7 +6113,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2006</v>
       </c>
@@ -6060,7 +6130,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2007</v>
       </c>
@@ -6077,7 +6147,7 @@
         <v>2.0055000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2008</v>
       </c>
@@ -6094,7 +6164,7 @@
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2009</v>
       </c>
@@ -6111,7 +6181,7 @@
         <v>1.0713999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2010</v>
       </c>
@@ -6128,7 +6198,7 @@
         <v>0.46700000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2011</v>
       </c>
@@ -6145,7 +6215,7 @@
         <v>0.2198</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2012</v>
       </c>
@@ -6162,7 +6232,7 @@
         <v>0.2747</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2013</v>
       </c>
@@ -6179,7 +6249,7 @@
         <v>0.1923</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2014</v>
       </c>
@@ -6196,7 +6266,7 @@
         <v>0.2198</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2015</v>
       </c>
@@ -6213,7 +6283,7 @@
         <v>0.24729999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2016</v>
       </c>
@@ -6230,7 +6300,7 @@
         <v>8.2400000000000001E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2017</v>
       </c>
@@ -6247,7 +6317,7 @@
         <v>0.24729999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2018</v>
       </c>
@@ -6264,7 +6334,7 @@
         <v>0.2747</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -6294,9 +6364,9 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6313,7 +6383,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1994</v>
       </c>
@@ -6330,7 +6400,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1995</v>
       </c>
@@ -6347,7 +6417,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1996</v>
       </c>
@@ -6364,7 +6434,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1997</v>
       </c>
@@ -6381,7 +6451,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1998</v>
       </c>
@@ -6398,7 +6468,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1999</v>
       </c>
@@ -6415,7 +6485,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2000</v>
       </c>
@@ -6432,7 +6502,7 @@
         <v>0.307</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -6449,7 +6519,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2002</v>
       </c>
@@ -6466,7 +6536,7 @@
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2003</v>
       </c>
@@ -6483,7 +6553,7 @@
         <v>0.21299999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2004</v>
       </c>
@@ -6500,7 +6570,7 @@
         <v>0.252</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2005</v>
       </c>
@@ -6517,7 +6587,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2006</v>
       </c>
@@ -6534,7 +6604,7 @@
         <v>0.23599999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2007</v>
       </c>
@@ -6551,7 +6621,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2008</v>
       </c>
@@ -6568,7 +6638,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2009</v>
       </c>
@@ -6585,7 +6655,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2010</v>
       </c>
@@ -6602,7 +6672,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2011</v>
       </c>
@@ -6619,7 +6689,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2012</v>
       </c>
@@ -6636,7 +6706,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2013</v>
       </c>
@@ -6653,7 +6723,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2014</v>
       </c>
@@ -6670,7 +6740,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2015</v>
       </c>
@@ -6687,7 +6757,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2016</v>
       </c>
@@ -6704,7 +6774,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2017</v>
       </c>
@@ -6721,7 +6791,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2018</v>
       </c>
@@ -6738,7 +6808,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>
@@ -6768,12 +6838,12 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6796,7 +6866,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1994</v>
       </c>
@@ -6819,7 +6889,7 @@
         <v>-1631.59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1995</v>
       </c>
@@ -6842,7 +6912,7 @@
         <v>-2465.64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1996</v>
       </c>
@@ -6865,7 +6935,7 @@
         <v>-6900.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1997</v>
       </c>
@@ -6888,7 +6958,7 @@
         <v>-3262.17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1998</v>
       </c>
@@ -6911,7 +6981,7 @@
         <v>-8541.9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1999</v>
       </c>
@@ -6934,7 +7004,7 @@
         <v>-4284.43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2000</v>
       </c>
@@ -6957,7 +7027,7 @@
         <v>-2235.08</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2001</v>
       </c>
@@ -6980,7 +7050,7 @@
         <v>-4070.58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2002</v>
       </c>
@@ -7003,7 +7073,7 @@
         <v>-4543.25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2003</v>
       </c>
@@ -7026,7 +7096,7 @@
         <v>-1977.03</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2004</v>
       </c>
@@ -7049,7 +7119,7 @@
         <v>-1247.9000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2005</v>
       </c>
@@ -7072,7 +7142,7 @@
         <v>-1890.97</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2006</v>
       </c>
@@ -7095,7 +7165,7 @@
         <v>-1704.28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2007</v>
       </c>
@@ -7118,7 +7188,7 @@
         <v>2441.66</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2008</v>
       </c>
@@ -7141,7 +7211,7 @@
         <v>673.15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2009</v>
       </c>
@@ -7164,7 +7234,7 @@
         <v>1707.8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>2010</v>
       </c>
@@ -7187,7 +7257,7 @@
         <v>1185.18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>2011</v>
       </c>
@@ -7210,7 +7280,7 @@
         <v>2911.45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>2012</v>
       </c>
@@ -7233,7 +7303,7 @@
         <v>2349.06</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2013</v>
       </c>
@@ -7256,7 +7326,7 @@
         <v>1880.07</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>2014</v>
       </c>
@@ -7279,7 +7349,7 @@
         <v>1473.18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>2015</v>
       </c>
@@ -7302,7 +7372,7 @@
         <v>2650.94</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2016</v>
       </c>
@@ -7325,7 +7395,7 @@
         <v>688.91</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2017</v>
       </c>
@@ -7348,7 +7418,7 @@
         <v>716.38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2018</v>
       </c>
@@ -7371,7 +7441,7 @@
         <v>1910.56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="23.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>